<commit_message>
Updated my Shopping list and a practical data analysis
</commit_message>
<xml_diff>
--- a/Microsoft Excel/Tanvir/Day 07.xlsx
+++ b/Microsoft Excel/Tanvir/Day 07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarato/Documents/GitHub/Spreadsheet/Microsoft Excel/Tanvir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C567035C-4876-1B40-AFFA-FAEA67AA84D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354DEB88-2C05-A34E-8A1C-1A3156CB88E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="2" xr2:uid="{15B3D749-4F2A-614D-9D42-67663B03A074}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t xml:space="preserve">FUNCTIONS </t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>grass</t>
+  </si>
+  <si>
+    <t>q</t>
   </si>
 </sst>
 </file>
@@ -1237,9 +1240,8 @@
       <c r="C9">
         <v>58</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="D9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>